<commit_message>
More scripting, PSPLIB->Excel converter first phase initial untested implementation
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreschnabel/Dropbox/Arbeit/SFB/Begehung/Begehungsdemo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.schnabel\Dropbox\Arbeit\SFB\Begehung\Begehungsdemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="460" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="13080" yWindow="465" windowWidth="28800" windowHeight="16695" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt 1" sheetId="1" r:id="rId1"/>
     <sheet name="Projekt 2" sheetId="2" r:id="rId2"/>
     <sheet name="Projekt 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Globals" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +32,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +66,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +100,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="21">
   <si>
     <t>Gesamt</t>
   </si>
@@ -182,6 +180,18 @@
   </si>
   <si>
     <t>Delaycost</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Kr_m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Kn_m</t>
   </si>
 </sst>
 </file>
@@ -642,7 +652,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1202,18 +1212,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1255,7 @@
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
     </row>
-    <row r="2" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1255,7 +1265,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>13</v>
       </c>
@@ -1293,7 +1303,7 @@
       <c r="AA3" s="38"/>
       <c r="AB3" s="38"/>
     </row>
-    <row r="4" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
@@ -1339,7 +1349,7 @@
       <c r="AA4" s="41"/>
       <c r="AB4" s="41"/>
     </row>
-    <row r="5" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43"/>
       <c r="C5" s="44"/>
@@ -1417,7 +1427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -1463,7 +1473,7 @@
       <c r="AA6" s="23"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>2</v>
       </c>
@@ -1505,7 +1515,7 @@
       <c r="AA7" s="14"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>3</v>
       </c>
@@ -1547,7 +1557,7 @@
       </c>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>4</v>
       </c>
@@ -1589,7 +1599,7 @@
       <c r="AA9" s="14"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>5</v>
       </c>
@@ -1633,7 +1643,7 @@
       <c r="AA10" s="14"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>6</v>
       </c>
@@ -1673,7 +1683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>7</v>
       </c>
@@ -1713,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>8</v>
       </c>
@@ -1753,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>9</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -1829,7 +1839,7 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1876,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1874,7 +1884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1906,18 +1916,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AB19"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E10" sqref="D9:E10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -1949,7 +1959,7 @@
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
     </row>
-    <row r="2" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1959,7 +1969,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>13</v>
       </c>
@@ -1997,7 +2007,7 @@
       <c r="AA3" s="38"/>
       <c r="AB3" s="38"/>
     </row>
-    <row r="4" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2053,7 @@
       <c r="AA4" s="41"/>
       <c r="AB4" s="41"/>
     </row>
-    <row r="5" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43"/>
       <c r="C5" s="44"/>
@@ -2121,7 +2131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -2167,7 +2177,7 @@
       <c r="AA6" s="23"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>2</v>
       </c>
@@ -2209,7 +2219,7 @@
       <c r="AA7" s="14"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>3</v>
       </c>
@@ -2251,7 +2261,7 @@
       </c>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>4</v>
       </c>
@@ -2293,7 +2303,7 @@
       <c r="AA9" s="14"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>5</v>
       </c>
@@ -2337,7 +2347,7 @@
       <c r="AA10" s="14"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>6</v>
       </c>
@@ -2377,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>7</v>
       </c>
@@ -2417,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>8</v>
       </c>
@@ -2457,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>9</v>
       </c>
@@ -2495,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -2533,7 +2543,7 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2580,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2578,7 +2588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2610,7 +2620,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:AB19"/>
@@ -2619,9 +2629,9 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -2653,7 +2663,7 @@
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
     </row>
-    <row r="2" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -2663,7 +2673,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>13</v>
       </c>
@@ -2701,7 +2711,7 @@
       <c r="AA3" s="38"/>
       <c r="AB3" s="38"/>
     </row>
-    <row r="4" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>9</v>
       </c>
@@ -2747,7 +2757,7 @@
       <c r="AA4" s="41"/>
       <c r="AB4" s="41"/>
     </row>
-    <row r="5" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42"/>
       <c r="B5" s="43"/>
       <c r="C5" s="44"/>
@@ -2825,7 +2835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -2871,7 +2881,7 @@
       <c r="AA6" s="23"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>2</v>
       </c>
@@ -2913,7 +2923,7 @@
       <c r="AA7" s="14"/>
       <c r="AB7" s="2"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>3</v>
       </c>
@@ -2955,7 +2965,7 @@
       </c>
       <c r="AB8" s="2"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>4</v>
       </c>
@@ -2997,7 +3007,7 @@
       <c r="AA9" s="14"/>
       <c r="AB9" s="2"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>5</v>
       </c>
@@ -3041,7 +3051,7 @@
       <c r="AA10" s="14"/>
       <c r="AB10" s="2"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>6</v>
       </c>
@@ -3081,7 +3091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>7</v>
       </c>
@@ -3121,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>8</v>
       </c>
@@ -3161,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>9</v>
       </c>
@@ -3199,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -3237,7 +3247,7 @@
       <c r="AA15" s="4"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
@@ -3274,7 +3284,7 @@
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3282,7 +3292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3310,4 +3320,47 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Show sequential and integrated optimization simultaneously Non draggable non overlapping layout
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt 1" sheetId="1" r:id="rId1"/>
@@ -934,7 +934,7 @@
   </sheetPr>
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3021,8 +3021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Watcher notify on start and finish of optimization - Show overtime capacity area correctly in schedule visualization, two horizontal limit lines (dashed red)
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreschnabel/Seafile/Dropbox/SFB/Begehung/Begehungsdemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF557E-5ABC-7948-9DB8-5FBDDF86C60B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820882F2-D73F-D542-918B-6AEB3CB78167}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15000" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="1820" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt 1" sheetId="1" r:id="rId1"/>
@@ -1031,22 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1089,17 +1074,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1388,41 +1388,41 @@
   <dimension ref="A1:AD44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB21" sqref="AB21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -1437,57 +1437,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="79" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="82" t="s">
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="73" t="s">
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="79"/>
+      <c r="AB3" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="74"/>
+      <c r="AC3" s="95"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="89" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -1496,44 +1496,44 @@
       <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="85" t="s">
+      <c r="H4" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="88" t="s">
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="75" t="s">
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="101" t="s">
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="90"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="85"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="AC5" s="70">
         <v>2</v>
       </c>
-      <c r="AD5" s="101"/>
+      <c r="AD5" s="71"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
@@ -2189,7 +2189,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="92" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
+      <c r="A24" s="92"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -2227,7 +2227,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="92" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -2245,7 +2245,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -2261,7 +2261,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="92"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="93" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="63">
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="72"/>
+      <c r="A33" s="93"/>
       <c r="B33" s="68">
         <v>13</v>
       </c>
@@ -2323,7 +2323,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="72"/>
+      <c r="A34" s="93"/>
       <c r="B34" s="64">
         <v>14</v>
       </c>
@@ -2358,7 +2358,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="72" t="s">
+      <c r="A37" s="93" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="63">
@@ -2375,7 +2375,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="72"/>
+      <c r="A38" s="93"/>
       <c r="B38" s="68">
         <v>13</v>
       </c>
@@ -2390,7 +2390,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="72"/>
+      <c r="A39" s="93"/>
       <c r="B39" s="64">
         <v>14</v>
       </c>
@@ -2425,7 +2425,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="72" t="s">
+      <c r="A42" s="93" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="63">
@@ -2442,7 +2442,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="72"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="68">
         <v>13</v>
       </c>
@@ -2457,7 +2457,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="72"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="64">
         <v>14</v>
       </c>
@@ -2473,6 +2473,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="E3:Q3"/>
@@ -2485,13 +2492,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="4">
@@ -2561,35 +2561,35 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -2617,57 +2617,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="96" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="82" t="s">
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="83"/>
-      <c r="AB3" s="73" t="s">
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="78"/>
+      <c r="AB3" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="74"/>
+      <c r="AC3" s="95"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="84" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="36" t="s">
@@ -2679,41 +2679,41 @@
       <c r="H4" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="97" t="s">
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="75" t="s">
+      <c r="S4" s="73"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
+      <c r="Z4" s="73"/>
+      <c r="AA4" s="73"/>
+      <c r="AB4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="101" t="s">
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -2786,7 +2786,7 @@
       <c r="AC5" s="70">
         <v>2</v>
       </c>
-      <c r="AD5" s="101"/>
+      <c r="AD5" s="71"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
@@ -3371,7 +3371,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="92" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -3391,7 +3391,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
+      <c r="A24" s="92"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="92" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -3427,7 +3427,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -3443,7 +3443,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="92"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -3460,6 +3460,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="R4:AA4"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="B3:D3"/>
@@ -3471,11 +3476,6 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:Q4"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="R4:AA4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="1">
@@ -3509,35 +3509,35 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
+      <c r="A1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -3552,57 +3552,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="96" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="82" t="s">
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="79"/>
+      <c r="R3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
-      <c r="Z3" s="83"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="73" t="s">
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="79"/>
+      <c r="AB3" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="74"/>
+      <c r="AC3" s="95"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="100" t="s">
+      <c r="D4" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="84" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -3611,44 +3611,44 @@
       <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="96" t="s">
+      <c r="H4" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="82" t="s">
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="83"/>
-      <c r="X4" s="83"/>
-      <c r="Y4" s="83"/>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="84"/>
-      <c r="AB4" s="75" t="s">
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="101" t="s">
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="71" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="91"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -3721,7 +3721,7 @@
       <c r="AC5" s="70">
         <v>2</v>
       </c>
-      <c r="AD5" s="101"/>
+      <c r="AD5" s="71"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="49">
@@ -4308,7 +4308,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="92" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -4328,7 +4328,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
+      <c r="A24" s="92"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="92" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -4364,7 +4364,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
+      <c r="A26" s="92"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -4380,7 +4380,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="92"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -4397,6 +4397,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="R4:AA4"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="B3:D3"/>
@@ -4408,11 +4413,6 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:Q4"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="R4:AA4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Sequential scheduling with quality consideration
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreschnabel/Seafile/Dropbox/SFB/Begehung/Begehungsdemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820882F2-D73F-D542-918B-6AEB3CB78167}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA53650-D321-944A-92FF-71FAA4C4EDD9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="1820" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16220" yWindow="440" windowWidth="22980" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt 1" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="37">
   <si>
     <t>Daten</t>
   </si>
@@ -187,25 +187,28 @@
     <t>zmax_r</t>
   </si>
   <si>
-    <t>Kunde P1</t>
-  </si>
-  <si>
-    <t>Kunde P2</t>
-  </si>
-  <si>
-    <t>Kunde P3</t>
-  </si>
-  <si>
     <t>Qualität</t>
   </si>
   <si>
     <t>q(j,o)</t>
   </si>
   <si>
-    <t>OC cost</t>
+    <t>c(j)</t>
   </si>
   <si>
-    <t>c(j)</t>
+    <t>kappa_r</t>
+  </si>
+  <si>
+    <t>Kapazität erneuerbar</t>
+  </si>
+  <si>
+    <t>Kapazität nicht-erneuerbar</t>
+  </si>
+  <si>
+    <t>Maximale Überstunden</t>
+  </si>
+  <si>
+    <t>Überstundenkosten</t>
   </si>
 </sst>
 </file>
@@ -911,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1024,11 +1027,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1074,34 +1089,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1385,44 +1385,44 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:AD44"/>
+  <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -1437,57 +1437,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="74" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="77" t="s">
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="79"/>
-      <c r="AB3" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="95"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="72"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="93" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -1496,44 +1496,44 @@
       <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="83" t="s">
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="86"/>
+      <c r="R4" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="81"/>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="71" t="s">
-        <v>35</v>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="75" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="85"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -1603,10 +1603,10 @@
       <c r="AB5" s="26">
         <v>1</v>
       </c>
-      <c r="AC5" s="70">
+      <c r="AC5" s="68">
         <v>2</v>
       </c>
-      <c r="AD5" s="71"/>
+      <c r="AD5" s="75"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
@@ -2163,13 +2163,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6">
-        <v>5</v>
-      </c>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2189,7 +2185,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="70" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -2209,7 +2205,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -2227,7 +2223,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="70" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -2245,7 +2241,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -2261,7 +2257,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -2276,210 +2272,15 @@
       </c>
       <c r="F27" s="33"/>
     </row>
-    <row r="30" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="63">
-        <v>12</v>
-      </c>
-      <c r="C32" s="50">
-        <v>50</v>
-      </c>
-      <c r="D32" s="65">
-        <v>40</v>
-      </c>
-      <c r="E32" s="51">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="93"/>
-      <c r="B33" s="68">
-        <v>13</v>
-      </c>
-      <c r="C33" s="66">
-        <v>49</v>
-      </c>
-      <c r="D33" s="38">
-        <v>39</v>
-      </c>
-      <c r="E33" s="67">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="93"/>
-      <c r="B34" s="64">
-        <v>14</v>
-      </c>
-      <c r="C34" s="52">
-        <v>48</v>
-      </c>
-      <c r="D34" s="34">
-        <v>38</v>
-      </c>
-      <c r="E34" s="53">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-    </row>
-    <row r="36" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="63">
-        <v>12</v>
-      </c>
-      <c r="C37" s="50">
-        <v>50</v>
-      </c>
-      <c r="D37" s="65">
-        <v>49</v>
-      </c>
-      <c r="E37" s="51">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="93"/>
-      <c r="B38" s="68">
-        <v>13</v>
-      </c>
-      <c r="C38" s="66">
-        <v>40</v>
-      </c>
-      <c r="D38" s="38">
-        <v>39</v>
-      </c>
-      <c r="E38" s="67">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93"/>
-      <c r="B39" s="64">
-        <v>14</v>
-      </c>
-      <c r="C39" s="52">
-        <v>30</v>
-      </c>
-      <c r="D39" s="34">
-        <v>29</v>
-      </c>
-      <c r="E39" s="53">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-    </row>
-    <row r="41" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="63">
-        <v>12</v>
-      </c>
-      <c r="C42" s="50">
-        <v>40</v>
-      </c>
-      <c r="D42" s="65">
-        <v>39</v>
-      </c>
-      <c r="E42" s="51">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93"/>
-      <c r="B43" s="68">
-        <v>13</v>
-      </c>
-      <c r="C43" s="66">
-        <v>39</v>
-      </c>
-      <c r="D43" s="38">
-        <v>38</v>
-      </c>
-      <c r="E43" s="67">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93"/>
-      <c r="B44" s="64">
-        <v>14</v>
-      </c>
-      <c r="C44" s="52">
-        <v>38</v>
-      </c>
-      <c r="D44" s="34">
-        <v>37</v>
-      </c>
-      <c r="E44" s="53">
-        <v>36</v>
-      </c>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="A23:A24"/>
+  <mergeCells count="16">
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="E3:Q3"/>
@@ -2492,45 +2293,13 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42:E44">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:E39">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:E34">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2554,42 +2323,42 @@
   </sheetPr>
   <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -2617,57 +2386,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="91" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="77" t="s">
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="95"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="72"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="88" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="36" t="s">
@@ -2676,44 +2445,44 @@
       <c r="G4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="98" t="s">
+      <c r="H4" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="99" t="s">
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="71" t="s">
-        <v>35</v>
+      <c r="S4" s="77"/>
+      <c r="T4" s="77"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
+      <c r="AA4" s="77"/>
+      <c r="AB4" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="75" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -2783,10 +2552,10 @@
       <c r="AB5" s="26">
         <v>1</v>
       </c>
-      <c r="AC5" s="70">
+      <c r="AC5" s="68">
         <v>2</v>
       </c>
-      <c r="AD5" s="71"/>
+      <c r="AD5" s="75"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="25">
@@ -3345,13 +3114,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6">
-        <v>5</v>
-      </c>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3371,7 +3136,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="70" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -3391,7 +3156,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -3409,7 +3174,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="70" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -3427,7 +3192,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -3443,7 +3208,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -3460,11 +3225,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="R4:AA4"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="B3:D3"/>
@@ -3476,6 +3236,11 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:Q4"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="R4:AA4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="1">
@@ -3502,42 +3267,42 @@
   </sheetPr>
   <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="S1" s="73"/>
-      <c r="T1" s="73"/>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="73"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32"/>
@@ -3552,57 +3317,57 @@
       <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="91" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="79"/>
-      <c r="R3" s="77" t="s">
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="79"/>
-      <c r="AB3" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="95"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="72"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E4" s="88" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="31" t="s">
@@ -3611,44 +3376,44 @@
       <c r="G4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="77" t="s">
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="71" t="s">
-        <v>35</v>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="82"/>
+      <c r="X4" s="82"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="82"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="75" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="86"/>
+      <c r="A5" s="98"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="90"/>
       <c r="F5" s="26">
         <v>1</v>
       </c>
@@ -3718,10 +3483,10 @@
       <c r="AB5" s="26">
         <v>1</v>
       </c>
-      <c r="AC5" s="70">
+      <c r="AC5" s="68">
         <v>2</v>
       </c>
-      <c r="AD5" s="71"/>
+      <c r="AD5" s="75"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="49">
@@ -4282,13 +4047,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6">
-        <v>5</v>
-      </c>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4308,7 +4069,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="92" t="s">
+      <c r="A23" s="70" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="47">
@@ -4328,7 +4089,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
+      <c r="A24" s="70"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -4346,7 +4107,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="70" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="47">
@@ -4364,7 +4125,7 @@
       <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="2">
         <v>13</v>
       </c>
@@ -4380,7 +4141,7 @@
       <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="1">
         <v>14</v>
       </c>
@@ -4397,11 +4158,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="R4:AA4"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="B3:D3"/>
@@ -4413,6 +4169,11 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:Q4"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="R4:AA4"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:E27">
     <cfRule type="colorScale" priority="1">
@@ -4434,16 +4195,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:J3"/>
+  <dimension ref="B1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
@@ -4463,8 +4237,14 @@
         <v>28</v>
       </c>
       <c r="J2" s="38"/>
-    </row>
-    <row r="3" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="101" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="102" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="56">
         <v>1</v>
       </c>
@@ -4484,6 +4264,12 @@
         <v>2</v>
       </c>
       <c r="J3" s="38"/>
+      <c r="K3" s="100">
+        <v>1</v>
+      </c>
+      <c r="L3" s="69">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>